<commit_message>
New version of the main executable: CriptoUpdateClasses.py
New Changes
Now there is frequency
</commit_message>
<xml_diff>
--- a/Portfólio.xlsx
+++ b/Portfólio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\Cripto_Update_0.9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30899152-4D41-4A1F-B6AC-091CFFB736DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF891F2-6BC1-4555-A8C8-9C3A7AE28003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3A04169C-532D-4034-AA99-2F4DEFE8AC13}"/>
+    <workbookView xWindow="6195" yWindow="2685" windowWidth="18900" windowHeight="11055" xr2:uid="{3A04169C-532D-4034-AA99-2F4DEFE8AC13}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Nome</t>
   </si>
@@ -40,6 +40,159 @@
   </si>
   <si>
     <t>Supply</t>
+  </si>
+  <si>
+    <t>Bitcoin</t>
+  </si>
+  <si>
+    <t>Binance Coin</t>
+  </si>
+  <si>
+    <t>153,432,897 BNB</t>
+  </si>
+  <si>
+    <t>Cardano</t>
+  </si>
+  <si>
+    <t>31,948,309,441 ADA</t>
+  </si>
+  <si>
+    <t>Litecoin</t>
+  </si>
+  <si>
+    <t>66,752,415 LTC</t>
+  </si>
+  <si>
+    <t>Chainlink</t>
+  </si>
+  <si>
+    <t>419,009,556 LINK</t>
+  </si>
+  <si>
+    <t>Dash</t>
+  </si>
+  <si>
+    <t>DODO</t>
+  </si>
+  <si>
+    <t>110,551,965 DODO</t>
+  </si>
+  <si>
+    <t>Olyseum</t>
+  </si>
+  <si>
+    <t>1,140,983,359 OLY</t>
+  </si>
+  <si>
+    <t>Crypterium</t>
+  </si>
+  <si>
+    <t>83,925,400 CRPT</t>
+  </si>
+  <si>
+    <t>Autonio</t>
+  </si>
+  <si>
+    <t>82,323,050 NIOX</t>
+  </si>
+  <si>
+    <t>Tether</t>
+  </si>
+  <si>
+    <t>EOS</t>
+  </si>
+  <si>
+    <t>PancakeSwap</t>
+  </si>
+  <si>
+    <t>Avalanche</t>
+  </si>
+  <si>
+    <t>Ren</t>
+  </si>
+  <si>
+    <t>997,163,051 REN</t>
+  </si>
+  <si>
+    <t>Badger DAO</t>
+  </si>
+  <si>
+    <t>8,603,194 BADGER</t>
+  </si>
+  <si>
+    <t>Ambrosus</t>
+  </si>
+  <si>
+    <t>55,536,494,298 USDT</t>
+  </si>
+  <si>
+    <t>953,236,428 EOS</t>
+  </si>
+  <si>
+    <t>164,900,129 CAKE</t>
+  </si>
+  <si>
+    <t>18,705,075 BTC</t>
+  </si>
+  <si>
+    <t>128,861,700 AVAX</t>
+  </si>
+  <si>
+    <t>10,122,818 DASH</t>
+  </si>
+  <si>
+    <t>180,931,869 AMB</t>
+  </si>
+  <si>
+    <t>$64,796,575,967  /  1,119,561 BTC</t>
+  </si>
+  <si>
+    <t>$4,341,251,493  /  6,540,125 BNB</t>
+  </si>
+  <si>
+    <t>$7,948,772,285  /  4,460,452,952 ADA</t>
+  </si>
+  <si>
+    <t>$175,692,319,180  /  175,672,930,468 USDT</t>
+  </si>
+  <si>
+    <t>$8,596,858,930  /  23,945,077 LTC</t>
+  </si>
+  <si>
+    <t>$2,893,037,275  /  56,595,772 LINK</t>
+  </si>
+  <si>
+    <t>$6,953,954,900  /  696,316,952 EOS</t>
+  </si>
+  <si>
+    <t>$451,848,205  /  11,688,026 CAKE</t>
+  </si>
+  <si>
+    <t>$314,734,251  /  8,218,191 AVAX</t>
+  </si>
+  <si>
+    <t>$1,206,322,452  /  3,051,542 DASH</t>
+  </si>
+  <si>
+    <t>$95,817,419  /  99,825,277 REN</t>
+  </si>
+  <si>
+    <t>$33,636,253  /  9,544,707 DODO</t>
+  </si>
+  <si>
+    <t>$51,845,242  /  1,464,275 BADGER</t>
+  </si>
+  <si>
+    <t>$420,116  /  1,306,175 CRPT</t>
+  </si>
+  <si>
+    <t>$44,394  /  2,115,319 OLY</t>
+  </si>
+  <si>
+    <t>$1,019,847  /  3,726,359 NIOX</t>
+  </si>
+  <si>
+    <t>$3,669,879  /  41,136,847 AMB</t>
   </si>
 </sst>
 </file>
@@ -406,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F077E40B-FF0B-4F63-A769-C644779E2C0C}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,52 +590,297 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>57876.77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>663.79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>359.02</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>51.12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.6399999999999996E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
+        <v>38.659999999999997</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>395.32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
       <c r="L11" s="3"/>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.95989999999999998</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
       <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.3216</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2">
+        <v>9.1200000000000003E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.0990000000000002E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.2737</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.9209999999999998E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1343</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>